<commit_message>
add seedData to services
</commit_message>
<xml_diff>
--- a/idea-hamster-profile-service/src/main/resources/ih-profile-service.xlsx
+++ b/idea-hamster-profile-service/src/main/resources/ih-profile-service.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">ideaHamster</t>
   </si>
   <si>
-    <t xml:space="preserve">Soumya@123</t>
+    <t xml:space="preserve">Soumya@1234</t>
   </si>
   <si>
     <t xml:space="preserve">kiran</t>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">kiran@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Kiran@123</t>
+    <t xml:space="preserve">Kiran@1234</t>
   </si>
   <si>
     <t xml:space="preserve">pratyusha</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">pratyusha@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Pratyusha@123</t>
+    <t xml:space="preserve">Pratyusha@1234</t>
   </si>
   <si>
     <t xml:space="preserve">shubha</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">shubha@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Shubha@123</t>
+    <t xml:space="preserve">Shubha@1234</t>
   </si>
   <si>
     <t xml:space="preserve">rajni</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">rajni@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Rajni@123</t>
+    <t xml:space="preserve">Rajni@1234</t>
   </si>
   <si>
     <t xml:space="preserve">akansha</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">akansha@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Akansha@123</t>
+    <t xml:space="preserve">Akansha@1234</t>
   </si>
   <si>
     <t xml:space="preserve">hindu</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">hindu@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Hindu@123</t>
+    <t xml:space="preserve">Hindu@1234</t>
   </si>
   <si>
     <t xml:space="preserve">bindu</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">bindu@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Bindu@123</t>
+    <t xml:space="preserve">Bindu@1234</t>
   </si>
   <si>
     <t xml:space="preserve">sindhu</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">sindhi@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Sindhu@123</t>
+    <t xml:space="preserve">Sindhu@1234</t>
   </si>
   <si>
     <t xml:space="preserve">nisha</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">nisha@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Nishi@123</t>
+    <t xml:space="preserve">Nishi@1234</t>
   </si>
   <si>
     <t xml:space="preserve">pallavi</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">pallavi@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Pallavi@123</t>
+    <t xml:space="preserve">Pallavi@1234</t>
   </si>
   <si>
     <t xml:space="preserve">harika</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">harika@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Harika@123</t>
+    <t xml:space="preserve">Harika@1234</t>
   </si>
   <si>
     <t xml:space="preserve">akhila</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">akhila@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Akhil@123</t>
+    <t xml:space="preserve">Akhil@1234</t>
   </si>
   <si>
     <t xml:space="preserve">monika</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">monika@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Monika@123</t>
+    <t xml:space="preserve">Monika@1234</t>
   </si>
   <si>
     <t xml:space="preserve">priyanka</t>
@@ -172,7 +172,7 @@
     <t xml:space="preserve">priyanka@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Priyanka@123</t>
+    <t xml:space="preserve">Priyanka@1234</t>
   </si>
   <si>
     <t xml:space="preserve">shradda</t>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">shradda@mail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Shradda@123</t>
+    <t xml:space="preserve">Shradda@1234</t>
   </si>
   <si>
     <t xml:space="preserve">nithya</t>
@@ -190,7 +190,7 @@
     <t xml:space="preserve">nithya@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Nithya@123</t>
+    <t xml:space="preserve">Nithya@1234</t>
   </si>
   <si>
     <t xml:space="preserve">poornima</t>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">poornima@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Poornima@123</t>
+    <t xml:space="preserve">Poornima@1234</t>
   </si>
   <si>
     <t xml:space="preserve">chethana</t>
@@ -208,7 +208,16 @@
     <t xml:space="preserve">chethana@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Chethana@123</t>
+    <t xml:space="preserve">Chethana@1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">akshar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">akshar@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akshar@123</t>
   </si>
 </sst>
 </file>
@@ -316,16 +325,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
@@ -654,7 +663,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>60</v>
       </c>
@@ -669,6 +678,23 @@
       </c>
       <c r="E20" s="1" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>8273827218</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -696,6 +722,8 @@
     <hyperlink ref="E19" r:id="rId21" display="Poornima@123"/>
     <hyperlink ref="B20" r:id="rId22" display="chethana@gmail.com"/>
     <hyperlink ref="E20" r:id="rId23" display="Chethana@123"/>
+    <hyperlink ref="B21" r:id="rId24" display="akshar@gmail.com"/>
+    <hyperlink ref="E21" r:id="rId25" display="Akshar@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
modified in front end
</commit_message>
<xml_diff>
--- a/idea-hamster-profile-service/src/main/resources/ih-profile-service.xlsx
+++ b/idea-hamster-profile-service/src/main/resources/ih-profile-service.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">soumya</t>
+    <t xml:space="preserve">Soumya</t>
   </si>
   <si>
     <t xml:space="preserve">soumya@gmail.com</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Soumya@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">kiran</t>
+    <t xml:space="preserve">Kiran</t>
   </si>
   <si>
     <t xml:space="preserve">kiran@gmail.com</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Kiran@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">pratyusha</t>
+    <t xml:space="preserve">Pratyusha</t>
   </si>
   <si>
     <t xml:space="preserve">pratyusha@gmail.com</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Pratyusha@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">shubha</t>
+    <t xml:space="preserve">Shubha</t>
   </si>
   <si>
     <t xml:space="preserve">shubha@gmail.com</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Shubha@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">rajni</t>
+    <t xml:space="preserve">Rajni</t>
   </si>
   <si>
     <t xml:space="preserve">rajni@gmail.com</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Rajni@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">akansha</t>
+    <t xml:space="preserve">Akansha</t>
   </si>
   <si>
     <t xml:space="preserve">akansha@gmail.com</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">Akansha@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">hindu</t>
+    <t xml:space="preserve">Hindu</t>
   </si>
   <si>
     <t xml:space="preserve">hindu@gmail.com</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Hindu@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">bindu</t>
+    <t xml:space="preserve">Bindu</t>
   </si>
   <si>
     <t xml:space="preserve">bindu@gmail.com</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Bindu@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">sindhu</t>
+    <t xml:space="preserve">Sindhu</t>
   </si>
   <si>
     <t xml:space="preserve">sindhi@gmail.com</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">Sindhu@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">nisha</t>
+    <t xml:space="preserve">Nisha</t>
   </si>
   <si>
     <t xml:space="preserve">nisha@gmail.com</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Nishi@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">pallavi</t>
+    <t xml:space="preserve">Pallavi</t>
   </si>
   <si>
     <t xml:space="preserve">pallavi@gmail.com</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Pallavi@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">harika</t>
+    <t xml:space="preserve">Harika</t>
   </si>
   <si>
     <t xml:space="preserve">harika@gmail.com</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Harika@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">akhila</t>
+    <t xml:space="preserve">Akhila</t>
   </si>
   <si>
     <t xml:space="preserve">akhila@gmail.com</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">Akhil@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">monika</t>
+    <t xml:space="preserve">Monika</t>
   </si>
   <si>
     <t xml:space="preserve">monika@gmail.com</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Monika@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">priyanka</t>
+    <t xml:space="preserve">Priyanka</t>
   </si>
   <si>
     <t xml:space="preserve">priyanka@gmail.com</t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">Priyanka@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">shradda</t>
+    <t xml:space="preserve">Shradda</t>
   </si>
   <si>
     <t xml:space="preserve">shradda@mail.com</t>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">Shradda@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">nithya</t>
+    <t xml:space="preserve">Nithya</t>
   </si>
   <si>
     <t xml:space="preserve">nithya@gmail.com</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">Nithya@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">poornima</t>
+    <t xml:space="preserve">Poornima</t>
   </si>
   <si>
     <t xml:space="preserve">poornima@gmail.com</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Poornima@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">chethana</t>
+    <t xml:space="preserve">Chethana</t>
   </si>
   <si>
     <t xml:space="preserve">chethana@gmail.com</t>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">Chethana@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">akshar</t>
+    <t xml:space="preserve">Akshar</t>
   </si>
   <si>
     <t xml:space="preserve">akshar@gmail.com</t>
@@ -328,7 +328,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -699,29 +699,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Soumya@123"/>
-    <hyperlink ref="E3" r:id="rId2" display="Kiran@123"/>
-    <hyperlink ref="E4" r:id="rId3" display="Pratyusha@123"/>
-    <hyperlink ref="E5" r:id="rId4" display="Shubha@123"/>
-    <hyperlink ref="E6" r:id="rId5" display="Rajni@123"/>
-    <hyperlink ref="E7" r:id="rId6" display="Akansha@123"/>
-    <hyperlink ref="E8" r:id="rId7" display="Hindu@123"/>
-    <hyperlink ref="E9" r:id="rId8" display="Bindu@123"/>
-    <hyperlink ref="E10" r:id="rId9" display="Sindhu@123"/>
-    <hyperlink ref="E11" r:id="rId10" display="Nishi@123"/>
-    <hyperlink ref="E12" r:id="rId11" display="Pallavi@123"/>
-    <hyperlink ref="E13" r:id="rId12" display="Harika@123"/>
-    <hyperlink ref="E14" r:id="rId13" display="Akhil@123"/>
-    <hyperlink ref="E15" r:id="rId14" display="Monika@123"/>
-    <hyperlink ref="E16" r:id="rId15" display="Priyanka@123"/>
+    <hyperlink ref="E2" r:id="rId1" display="Soumya@1234"/>
+    <hyperlink ref="E3" r:id="rId2" display="Kiran@1234"/>
+    <hyperlink ref="E4" r:id="rId3" display="Pratyusha@1234"/>
+    <hyperlink ref="E5" r:id="rId4" display="Shubha@1234"/>
+    <hyperlink ref="E6" r:id="rId5" display="Rajni@1234"/>
+    <hyperlink ref="E7" r:id="rId6" display="Akansha@1234"/>
+    <hyperlink ref="E8" r:id="rId7" display="Hindu@1234"/>
+    <hyperlink ref="E9" r:id="rId8" display="Bindu@1234"/>
+    <hyperlink ref="E10" r:id="rId9" display="Sindhu@1234"/>
+    <hyperlink ref="E11" r:id="rId10" display="Nishi@1234"/>
+    <hyperlink ref="E12" r:id="rId11" display="Pallavi@1234"/>
+    <hyperlink ref="E13" r:id="rId12" display="Harika@1234"/>
+    <hyperlink ref="E14" r:id="rId13" display="Akhil@1234"/>
+    <hyperlink ref="E15" r:id="rId14" display="Monika@1234"/>
+    <hyperlink ref="E16" r:id="rId15" display="Priyanka@1234"/>
     <hyperlink ref="B17" r:id="rId16" display="shradda@mail.com"/>
-    <hyperlink ref="E17" r:id="rId17" display="Shradda@123"/>
+    <hyperlink ref="E17" r:id="rId17" display="Shradda@1234"/>
     <hyperlink ref="B18" r:id="rId18" display="nithya@gmail.com"/>
-    <hyperlink ref="E18" r:id="rId19" display="Nithya@123"/>
+    <hyperlink ref="E18" r:id="rId19" display="Nithya@1234"/>
     <hyperlink ref="B19" r:id="rId20" display="poornima@gmail.com"/>
-    <hyperlink ref="E19" r:id="rId21" display="Poornima@123"/>
+    <hyperlink ref="E19" r:id="rId21" display="Poornima@1234"/>
     <hyperlink ref="B20" r:id="rId22" display="chethana@gmail.com"/>
-    <hyperlink ref="E20" r:id="rId23" display="Chethana@123"/>
+    <hyperlink ref="E20" r:id="rId23" display="Chethana@1234"/>
     <hyperlink ref="B21" r:id="rId24" display="akshar@gmail.com"/>
     <hyperlink ref="E21" r:id="rId25" display="Akshar@123"/>
   </hyperlinks>

</xml_diff>